<commit_message>
Data Tables & Report Types
performed data manipulation for use in the report creation.
Also added 2 categories of report(source and Meter).
</commit_message>
<xml_diff>
--- a/raw.simulated.xlsx
+++ b/raw.simulated.xlsx
@@ -11,6 +11,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results1" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results2" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results3" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results4" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14078,4 +14079,653 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.000000115199599</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.802489578389735e-07</v>
+      </c>
+      <c r="D2" t="n">
+        <v>60.77165363304854</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.000000085199701</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.037169294434598e-07</v>
+      </c>
+      <c r="D3" t="n">
+        <v>239.6498244792372</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.000000129499554</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.946368596048873e-07</v>
+      </c>
+      <c r="D4" t="n">
+        <v>58.86919988957849</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1.000000162499445</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.107040979064427e-07</v>
+      </c>
+      <c r="D5" t="n">
+        <v>262.6782845453528</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.9999999307998931</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.59463771832785e-07</v>
+      </c>
+      <c r="D6" t="n">
+        <v>72.14539649239393</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-0.999995873330345</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.691640071706808e-07</v>
+      </c>
+      <c r="D7" t="n">
+        <v>39.93147396742826</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.999999804499721</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.976469793833022e-07</v>
+      </c>
+      <c r="D8" t="n">
+        <v>59.9601253263599</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-0.9999952072652042</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.162357639851018e-07</v>
+      </c>
+      <c r="D9" t="n">
+        <v>224.4808944000997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1.000000179699368</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.758458168828267e-07</v>
+      </c>
+      <c r="D11" t="n">
+        <v>72.27050017091349</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1.000000280699042</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1.110531291338026e-07</v>
+      </c>
+      <c r="D12" t="n">
+        <v>288.3458450289374</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1.000000090099679</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1.536305343423947e-07</v>
+      </c>
+      <c r="D13" t="n">
+        <v>86.79421766646065</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1.000000211099274</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1.166990425349784e-07</v>
+      </c>
+      <c r="D14" t="n">
+        <v>196.8927188940392</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.9999999502999158</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1.92447610844496e-07</v>
+      </c>
+      <c r="D15" t="n">
+        <v>65.71126121179844</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.9999976948012786</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1.305783916793309e-07</v>
+      </c>
+      <c r="D16" t="n">
+        <v>121.470969381151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.9999997788996681</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.549042305456387e-07</v>
+      </c>
+      <c r="D17" t="n">
+        <v>88.62942475753323</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.999997437402149</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1.2401858411045e-07</v>
+      </c>
+      <c r="D18" t="n">
+        <v>170.3420566652628</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1.000000234199192</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1.803895010871572e-07</v>
+      </c>
+      <c r="D20" t="n">
+        <v>56.9846951498985</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1.000000245199157</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1.070101237059364e-07</v>
+      </c>
+      <c r="D21" t="n">
+        <v>164.9968331489063</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1.000000250099158</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1.787892784402573e-07</v>
+      </c>
+      <c r="D22" t="n">
+        <v>65.13798623499994</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1.000000185099365</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1.032890878237564e-07</v>
+      </c>
+      <c r="D23" t="n">
+        <v>236.4814972049221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.9999998277997184</v>
+      </c>
+      <c r="C24" t="n">
+        <v>2.114240391005456e-07</v>
+      </c>
+      <c r="D24" t="n">
+        <v>47.72950892409442</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" t="n">
+        <v>-0.9999955163320013</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1.704910451572515e-07</v>
+      </c>
+      <c r="D25" t="n">
+        <v>40.656195462486</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.9999997288995974</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1.992771857571445e-07</v>
+      </c>
+      <c r="D26" t="n">
+        <v>57.68588286012108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" t="n">
+        <v>-0.9999952046645888</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1.084802822000873e-07</v>
+      </c>
+      <c r="D27" t="n">
+        <v>194.7535176245366</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.9999999496001796</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1.770219584173688e-07</v>
+      </c>
+      <c r="D29" t="n">
+        <v>65.20077483347286</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1.00000007859973</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1.015747466661297e-07</v>
+      </c>
+      <c r="D30" t="n">
+        <v>252.3248066679277</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1.000000048699826</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1.853213095933744e-07</v>
+      </c>
+      <c r="D31" t="n">
+        <v>58.3507749330185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1.000000221699248</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1.304853622856635e-07</v>
+      </c>
+      <c r="D32" t="n">
+        <v>155.8349103367076</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1.000000148400253</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1.952902691935279e-07</v>
+      </c>
+      <c r="D33" t="n">
+        <v>57.7929468030913</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0.9999977639015309</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1.229009290988736e-07</v>
+      </c>
+      <c r="D34" t="n">
+        <v>99.79788326084584</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0.9999998622997882</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1.913633567064056e-07</v>
+      </c>
+      <c r="D35" t="n">
+        <v>61.69637188242839</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0.9999974278023107</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1.281969502311858e-07</v>
+      </c>
+      <c r="D36" t="n">
+        <v>188.2229494523031</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" t="n">
+        <v>1.000000107999628</v>
+      </c>
+      <c r="C38" t="n">
+        <v>2.160434004477784e-07</v>
+      </c>
+      <c r="D38" t="n">
+        <v>43.12560146172058</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" t="n">
+        <v>1.000000159999457</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1.210580268479117e-07</v>
+      </c>
+      <c r="D39" t="n">
+        <v>125.3862465111772</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" t="n">
+        <v>1.000000123099571</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1.77581421798289e-07</v>
+      </c>
+      <c r="D40" t="n">
+        <v>58.8943255673224</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1.000000135099531</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1.117123948813383e-07</v>
+      </c>
+      <c r="D41" t="n">
+        <v>138.5010672008523</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0.9999999579999321</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1.550402105139492e-07</v>
+      </c>
+      <c r="D42" t="n">
+        <v>71.74320892045513</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43" t="n">
+        <v>-0.9999957315311693</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1.738697927153837e-07</v>
+      </c>
+      <c r="D43" t="n">
+        <v>43.81647763239668</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.9999998528997702</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1.709487018882085e-07</v>
+      </c>
+      <c r="D44" t="n">
+        <v>67.66508538814477</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" t="n">
+        <v>-0.9999951896649136</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1.09259134720857e-07</v>
+      </c>
+      <c r="D45" t="n">
+        <v>200.7045627732721</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>